<commit_message>
All files created (yay!)
</commit_message>
<xml_diff>
--- a/Tracking spreadsheet/Tracking spreadsheet.xlsx
+++ b/Tracking spreadsheet/Tracking spreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>File</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>Welcome to Jury Service</t>
+  </si>
+  <si>
+    <t>aboutus.html</t>
+  </si>
+  <si>
+    <t>panellookup2.html</t>
+  </si>
+  <si>
+    <t>panellookup3.html</t>
   </si>
 </sst>
 </file>
@@ -332,8 +341,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -437,7 +496,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="145">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -485,6 +544,31 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -532,6 +616,31 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -861,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -955,6 +1064,9 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1">
       <c r="B6" t="s">
@@ -1274,6 +1386,9 @@
       <c r="D30" t="s">
         <v>4</v>
       </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1">
       <c r="A31" t="s">
@@ -1282,6 +1397,12 @@
       <c r="C31" t="s">
         <v>41</v>
       </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1">
       <c r="B32" t="s">
@@ -1290,6 +1411,12 @@
       <c r="C32" t="s">
         <v>43</v>
       </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1">
       <c r="B33" t="s">
@@ -1298,6 +1425,12 @@
       <c r="C33" t="s">
         <v>45</v>
       </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" customHeight="1">
       <c r="B34" t="s">
@@ -1395,6 +1528,15 @@
       <c r="A41" t="s">
         <v>59</v>
       </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="12.75" customHeight="1">
       <c r="A42" t="s">
@@ -1406,6 +1548,9 @@
       <c r="D42" t="s">
         <v>4</v>
       </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="12.75" customHeight="1">
       <c r="A43" t="s">
@@ -1415,6 +1560,31 @@
         <v>63</v>
       </c>
       <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="12.75" customHeight="1">
+      <c r="C44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="12.75" customHeight="1">
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>